<commit_message>
fix excel data issues
</commit_message>
<xml_diff>
--- a/scripts/TenantSetup/TenantHttpData/driveItem/raptorWorkbookDriveItem.xlsx
+++ b/scripts/TenantSetup/TenantHttpData/driveItem/raptorWorkbookDriveItem.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24331"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_5D023280825A0CF6433B9BC9C1459C011EC968D0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F4E8CC3-1E13-4829-BC7B-26E16BFA535D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153D1657-2E65-489C-A121-E89744EFF767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -257,13 +257,16 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>UsedRange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,7 +310,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1222,24 +1252,40 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="MOD Administrator" id="{6373BEF4-F481-4B93-B140-7ADA2D1EA525}" userId="S::admin@m365x205864.onmicrosoft.com::97a13b0c-1678-4b7b-9bd2-4a80680f6bfa" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I14" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowCount="1" headerRowDxfId="16">
   <autoFilter ref="A1:I14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SSN" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Bank Account number" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Card Type" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Credit card number" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Title" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Department" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Approval Required"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Purchasing Office"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="8">
+      <totalsRowFormula>SUM(A2:A14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SSN" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="7">
+      <totalsRowFormula>SUM(B2:B14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Bank Account number" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="6">
+      <totalsRowFormula>SUM(C2:C14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Card Type" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5">
+      <totalsRowFormula>SUM(D2:D14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Credit card number" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="4">
+      <totalsRowFormula>SUM(E2:E14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Title" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="3">
+      <totalsRowFormula>SUM(F2:F14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Department" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="2">
+      <totalsRowFormula>SUM(G2:G14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Approval Required" totalsRowFunction="custom" totalsRowDxfId="1">
+      <totalsRowFormula>SUM(H2:H14)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Purchasing Office" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(I2:I14)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1508,11 +1554,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A15" dT="2021-07-13T19:17:02.43" personId="{6373BEF4-F481-4B93-B140-7ADA2D1EA525}" id="{9ED94D4D-E8A6-4EBE-9CB1-BAA7B80CBBCB}">
+  <threadedComment ref="A15" dT="2021-07-13T19:17:02.43" personId="{00000000-0000-0000-0000-000000000000}" id="{9ED94D4D-E8A6-4EBE-9CB1-BAA7B80CBBCB}">
     <text xml:space="preserve">Hello World
 </text>
   </threadedComment>
-  <threadedComment ref="A15" dT="2021-08-03T14:59:15.48" personId="{6373BEF4-F481-4B93-B140-7ADA2D1EA525}" id="{0081D753-28BA-457F-891D-9F3284E8EC78}" parentId="{9ED94D4D-E8A6-4EBE-9CB1-BAA7B80CBBCB}">
+  <threadedComment ref="A15" dT="2021-08-03T14:59:15.48" personId="{00000000-0000-0000-0000-000000000000}" id="{0081D753-28BA-457F-891D-9F3284E8EC78}" parentId="{9ED94D4D-E8A6-4EBE-9CB1-BAA7B80CBBCB}">
     <text>And to you all as well</text>
   </threadedComment>
 </ThreadedComments>
@@ -1523,10 +1569,10 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -1539,7 +1585,7 @@
     <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1597,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1626,7 +1672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1655,7 +1701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1684,7 +1730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1713,7 +1759,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1742,7 +1788,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -1771,7 +1817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1800,7 +1846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -1829,7 +1875,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1858,7 +1904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1887,7 +1933,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1916,7 +1962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>65</v>
       </c>
@@ -1945,25 +1991,56 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f>SUM(A2:A14)</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" ref="B15:I15" si="0">SUM(B2:B14)</f>
+        <v>5797035739</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>6.413578182487432E+16</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1972,7 +2049,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1981,7 +2058,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2052,6 +2129,27 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="bfbb771a-fb7a-4ea5-900b-dfb43202c772">EHSTRNS327EX-145-62</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="bfbb771a-fb7a-4ea5-900b-dfb43202c772">
+      <Url>https://3sharponline.sharepoint.com/sites/projects/compliancedemo/_layouts/15/DocIdRedir.aspx?ID=EHSTRNS327EX-145-62</Url>
+      <Description>EHSTRNS327EX-145-62</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035A5D6101F1B12428448D5A7936A43C4" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5171b377257429282e4574e5fb635aec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bfbb771a-fb7a-4ea5-900b-dfb43202c772" xmlns:ns3="b9b6af17-e42f-49ab-b438-b513461806fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dcc63583ae3daa245e8ce51837f20971" ns2:_="" ns3:_="">
     <xsd:import namespace="bfbb771a-fb7a-4ea5-900b-dfb43202c772"/>
@@ -2235,39 +2333,47 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="bfbb771a-fb7a-4ea5-900b-dfb43202c772">EHSTRNS327EX-145-62</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="bfbb771a-fb7a-4ea5-900b-dfb43202c772">
-      <Url>https://3sharponline.sharepoint.com/sites/projects/compliancedemo/_layouts/15/DocIdRedir.aspx?ID=EHSTRNS327EX-145-62</Url>
-      <Description>EHSTRNS327EX-145-62</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BE9B0B-A128-4786-93BD-CAD9E7C1A495}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BE9B0B-A128-4786-93BD-CAD9E7C1A495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26595CF2-E783-4FB7-91B5-E8B5DA6914E1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F92F9CAB-F563-424B-A2EC-0BE72C6E218A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D355177-F290-4A21-B52D-1472456111DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D355177-F290-4A21-B52D-1472456111DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bfbb771a-fb7a-4ea5-900b-dfb43202c772"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F92F9CAB-F563-424B-A2EC-0BE72C6E218A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26595CF2-E783-4FB7-91B5-E8B5DA6914E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bfbb771a-fb7a-4ea5-900b-dfb43202c772"/>
+    <ds:schemaRef ds:uri="b9b6af17-e42f-49ab-b438-b513461806fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>